<commit_message>
Submit the honour thesis
</commit_message>
<xml_diff>
--- a/Users/UsersFlow.xlsx
+++ b/Users/UsersFlow.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -95,37 +95,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1">
-                  <a:lumMod val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -212,7 +182,7 @@
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
-              <c:ptCount val="93"/>
+              <c:ptCount val="42"/>
               <c:pt idx="0">
                 <c:v>2010.7</c:v>
               </c:pt>
@@ -268,7 +238,7 @@
                 <c:v>12.0</c:v>
               </c:pt>
               <c:pt idx="18">
-                <c:v>2011.1</c:v>
+                <c:v>2012.1</c:v>
               </c:pt>
               <c:pt idx="19">
                 <c:v>2.0</c:v>
@@ -304,7 +274,7 @@
                 <c:v>12.0</c:v>
               </c:pt>
               <c:pt idx="30">
-                <c:v>2012.1</c:v>
+                <c:v>2013.1</c:v>
               </c:pt>
               <c:pt idx="31">
                 <c:v>2.0</c:v>
@@ -338,168 +308,15 @@
               </c:pt>
               <c:pt idx="41">
                 <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="42">
-                <c:v>2013.1</c:v>
-              </c:pt>
-              <c:pt idx="43">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="44">
-                <c:v>3.0</c:v>
-              </c:pt>
-              <c:pt idx="45">
-                <c:v>4.0</c:v>
-              </c:pt>
-              <c:pt idx="46">
-                <c:v>5.0</c:v>
-              </c:pt>
-              <c:pt idx="47">
-                <c:v>6.0</c:v>
-              </c:pt>
-              <c:pt idx="48">
-                <c:v>7.0</c:v>
-              </c:pt>
-              <c:pt idx="49">
-                <c:v>8.0</c:v>
-              </c:pt>
-              <c:pt idx="50">
-                <c:v>9.0</c:v>
-              </c:pt>
-              <c:pt idx="51">
-                <c:v>10.0</c:v>
-              </c:pt>
-              <c:pt idx="52">
-                <c:v>11.0</c:v>
-              </c:pt>
-              <c:pt idx="53">
-                <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="54">
-                <c:v>2014.1</c:v>
-              </c:pt>
-              <c:pt idx="55">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="56">
-                <c:v>3.0</c:v>
-              </c:pt>
-              <c:pt idx="57">
-                <c:v>4.0</c:v>
-              </c:pt>
-              <c:pt idx="58">
-                <c:v>5.0</c:v>
-              </c:pt>
-              <c:pt idx="59">
-                <c:v>6.0</c:v>
-              </c:pt>
-              <c:pt idx="60">
-                <c:v>7.0</c:v>
-              </c:pt>
-              <c:pt idx="61">
-                <c:v>8.0</c:v>
-              </c:pt>
-              <c:pt idx="62">
-                <c:v>9.0</c:v>
-              </c:pt>
-              <c:pt idx="63">
-                <c:v>10.0</c:v>
-              </c:pt>
-              <c:pt idx="64">
-                <c:v>11.0</c:v>
-              </c:pt>
-              <c:pt idx="65">
-                <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="66">
-                <c:v>2015.1</c:v>
-              </c:pt>
-              <c:pt idx="67">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="68">
-                <c:v>3.0</c:v>
-              </c:pt>
-              <c:pt idx="69">
-                <c:v>4.0</c:v>
-              </c:pt>
-              <c:pt idx="70">
-                <c:v>5.0</c:v>
-              </c:pt>
-              <c:pt idx="71">
-                <c:v>6.0</c:v>
-              </c:pt>
-              <c:pt idx="72">
-                <c:v>7.0</c:v>
-              </c:pt>
-              <c:pt idx="73">
-                <c:v>8.0</c:v>
-              </c:pt>
-              <c:pt idx="74">
-                <c:v>9.0</c:v>
-              </c:pt>
-              <c:pt idx="75">
-                <c:v>10.0</c:v>
-              </c:pt>
-              <c:pt idx="76">
-                <c:v>11.0</c:v>
-              </c:pt>
-              <c:pt idx="77">
-                <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="78">
-                <c:v>2016.1</c:v>
-              </c:pt>
-              <c:pt idx="79">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="80">
-                <c:v>3.0</c:v>
-              </c:pt>
-              <c:pt idx="81">
-                <c:v>4.0</c:v>
-              </c:pt>
-              <c:pt idx="82">
-                <c:v>5.0</c:v>
-              </c:pt>
-              <c:pt idx="83">
-                <c:v>6.0</c:v>
-              </c:pt>
-              <c:pt idx="84">
-                <c:v>7.0</c:v>
-              </c:pt>
-              <c:pt idx="85">
-                <c:v>8.0</c:v>
-              </c:pt>
-              <c:pt idx="86">
-                <c:v>9.0</c:v>
-              </c:pt>
-              <c:pt idx="87">
-                <c:v>10.0</c:v>
-              </c:pt>
-              <c:pt idx="88">
-                <c:v>11.0</c:v>
-              </c:pt>
-              <c:pt idx="89">
-                <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="90">
-                <c:v>2017.1</c:v>
-              </c:pt>
-              <c:pt idx="91">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="92">
-                <c:v>3.0</c:v>
               </c:pt>
             </c:numLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$A$1:$A$81</c:f>
+              <c:f>工作表1!$A$1:$A$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -528,7 +345,7 @@
                   <c:v>325.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>215.0</c:v>
+                  <c:v>214.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>226.0</c:v>
@@ -552,7 +369,7 @@
                   <c:v>345.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>292.0</c:v>
+                  <c:v>291.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>394.0</c:v>
@@ -615,7 +432,7 @@
                   <c:v>310.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>350.0</c:v>
+                  <c:v>349.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>352.0</c:v>
@@ -625,123 +442,6 @@
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>361.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>361.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>328.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>349.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>320.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>312.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>306.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>315.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>284.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>311.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>321.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>324.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>352.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>339.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>302.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>463.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3280.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1512.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1517.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>1422.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>1240.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1713.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>1490.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1533.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>1464.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1606.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>1702.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1841.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>2080.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1715.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1730.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1733.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1928.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>2633.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>4367.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>3360.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>2948.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>3002.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>3155.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1298.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,7 +529,7 @@
           <c:cat>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
-              <c:ptCount val="93"/>
+              <c:ptCount val="42"/>
               <c:pt idx="0">
                 <c:v>2010.7</c:v>
               </c:pt>
@@ -885,7 +585,7 @@
                 <c:v>12.0</c:v>
               </c:pt>
               <c:pt idx="18">
-                <c:v>2011.1</c:v>
+                <c:v>2012.1</c:v>
               </c:pt>
               <c:pt idx="19">
                 <c:v>2.0</c:v>
@@ -921,7 +621,7 @@
                 <c:v>12.0</c:v>
               </c:pt>
               <c:pt idx="30">
-                <c:v>2012.1</c:v>
+                <c:v>2013.1</c:v>
               </c:pt>
               <c:pt idx="31">
                 <c:v>2.0</c:v>
@@ -955,410 +655,140 @@
               </c:pt>
               <c:pt idx="41">
                 <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="42">
-                <c:v>2013.1</c:v>
-              </c:pt>
-              <c:pt idx="43">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="44">
-                <c:v>3.0</c:v>
-              </c:pt>
-              <c:pt idx="45">
-                <c:v>4.0</c:v>
-              </c:pt>
-              <c:pt idx="46">
-                <c:v>5.0</c:v>
-              </c:pt>
-              <c:pt idx="47">
-                <c:v>6.0</c:v>
-              </c:pt>
-              <c:pt idx="48">
-                <c:v>7.0</c:v>
-              </c:pt>
-              <c:pt idx="49">
-                <c:v>8.0</c:v>
-              </c:pt>
-              <c:pt idx="50">
-                <c:v>9.0</c:v>
-              </c:pt>
-              <c:pt idx="51">
-                <c:v>10.0</c:v>
-              </c:pt>
-              <c:pt idx="52">
-                <c:v>11.0</c:v>
-              </c:pt>
-              <c:pt idx="53">
-                <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="54">
-                <c:v>2014.1</c:v>
-              </c:pt>
-              <c:pt idx="55">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="56">
-                <c:v>3.0</c:v>
-              </c:pt>
-              <c:pt idx="57">
-                <c:v>4.0</c:v>
-              </c:pt>
-              <c:pt idx="58">
-                <c:v>5.0</c:v>
-              </c:pt>
-              <c:pt idx="59">
-                <c:v>6.0</c:v>
-              </c:pt>
-              <c:pt idx="60">
-                <c:v>7.0</c:v>
-              </c:pt>
-              <c:pt idx="61">
-                <c:v>8.0</c:v>
-              </c:pt>
-              <c:pt idx="62">
-                <c:v>9.0</c:v>
-              </c:pt>
-              <c:pt idx="63">
-                <c:v>10.0</c:v>
-              </c:pt>
-              <c:pt idx="64">
-                <c:v>11.0</c:v>
-              </c:pt>
-              <c:pt idx="65">
-                <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="66">
-                <c:v>2015.1</c:v>
-              </c:pt>
-              <c:pt idx="67">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="68">
-                <c:v>3.0</c:v>
-              </c:pt>
-              <c:pt idx="69">
-                <c:v>4.0</c:v>
-              </c:pt>
-              <c:pt idx="70">
-                <c:v>5.0</c:v>
-              </c:pt>
-              <c:pt idx="71">
-                <c:v>6.0</c:v>
-              </c:pt>
-              <c:pt idx="72">
-                <c:v>7.0</c:v>
-              </c:pt>
-              <c:pt idx="73">
-                <c:v>8.0</c:v>
-              </c:pt>
-              <c:pt idx="74">
-                <c:v>9.0</c:v>
-              </c:pt>
-              <c:pt idx="75">
-                <c:v>10.0</c:v>
-              </c:pt>
-              <c:pt idx="76">
-                <c:v>11.0</c:v>
-              </c:pt>
-              <c:pt idx="77">
-                <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="78">
-                <c:v>2016.1</c:v>
-              </c:pt>
-              <c:pt idx="79">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="80">
-                <c:v>3.0</c:v>
-              </c:pt>
-              <c:pt idx="81">
-                <c:v>4.0</c:v>
-              </c:pt>
-              <c:pt idx="82">
-                <c:v>5.0</c:v>
-              </c:pt>
-              <c:pt idx="83">
-                <c:v>6.0</c:v>
-              </c:pt>
-              <c:pt idx="84">
-                <c:v>7.0</c:v>
-              </c:pt>
-              <c:pt idx="85">
-                <c:v>8.0</c:v>
-              </c:pt>
-              <c:pt idx="86">
-                <c:v>9.0</c:v>
-              </c:pt>
-              <c:pt idx="87">
-                <c:v>10.0</c:v>
-              </c:pt>
-              <c:pt idx="88">
-                <c:v>11.0</c:v>
-              </c:pt>
-              <c:pt idx="89">
-                <c:v>12.0</c:v>
-              </c:pt>
-              <c:pt idx="90">
-                <c:v>2017.1</c:v>
-              </c:pt>
-              <c:pt idx="91">
-                <c:v>2.0</c:v>
-              </c:pt>
-              <c:pt idx="92">
-                <c:v>3.0</c:v>
               </c:pt>
             </c:numLit>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>工作表1!$B$1:$B$81</c:f>
+              <c:f>工作表1!$B$1:$B$42</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="81"/>
+                <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.0</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>32.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>64.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>80.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>126.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>79.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>92.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>99.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>126.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>118.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>106.0</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>86.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>111.0</c:v>
-                </c:pt>
                 <c:pt idx="19">
-                  <c:v>105.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>101.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>95.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>83.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>65.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>149.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>121.0</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>88.0</c:v>
+                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>171.0</c:v>
+                  <c:v>72.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>142.0</c:v>
+                  <c:v>59.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>105.0</c:v>
+                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>98.0</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>104.0</c:v>
+                  <c:v>54.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>120.0</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>116.0</c:v>
+                  <c:v>56.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>138.0</c:v>
+                  <c:v>66.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>141.0</c:v>
+                  <c:v>71.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>139.0</c:v>
+                  <c:v>72.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>159.0</c:v>
+                  <c:v>77.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>168.0</c:v>
+                  <c:v>87.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>175.0</c:v>
+                  <c:v>82.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>193.0</c:v>
+                  <c:v>82.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>134.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>162.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>157.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>151.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>136.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>141.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>135.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>145.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>114.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>134.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>146.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>128.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>136.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>127.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>122.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>251.0</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>2749.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>1119.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>1109.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>986.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>874.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>1268.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>1044.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1048.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>959.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>1126.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>1104.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>1169.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>1308.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>1000.0</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>1040.0</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>995.0</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>1108.0</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>1243.0</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>2695.0</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>1452.0</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>1193.0</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>1091.0</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>1235.0</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>477.0</c:v>
+                  <c:v>73.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1375,11 +805,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2091410128"/>
-        <c:axId val="-2106641792"/>
+        <c:axId val="-1760053520"/>
+        <c:axId val="-1760048400"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2091410128"/>
+        <c:axId val="-1760053520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,7 +856,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="lt1">
                     <a:lumMod val="75000"/>
@@ -1440,7 +870,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2106641792"/>
+        <c:crossAx val="-1760048400"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1448,7 +878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2106641792"/>
+        <c:axId val="-1760048400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,7 +938,941 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2091410128"/>
+        <c:crossAx val="-1760053520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="44"/>
+              <c:pt idx="0">
+                <c:v>2014.1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2.0</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3.0</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4.0</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6.0</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7.0</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8.0</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9.0</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11.0</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12.0</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>2015.1</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>2.0</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>3.0</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>4.0</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>6.0</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>7.0</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>8.0</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>9.0</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>11.0</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>12.0</c:v>
+              </c:pt>
+              <c:pt idx="24">
+                <c:v>2016.1</c:v>
+              </c:pt>
+              <c:pt idx="25">
+                <c:v>2.0</c:v>
+              </c:pt>
+              <c:pt idx="26">
+                <c:v>3.0</c:v>
+              </c:pt>
+              <c:pt idx="27">
+                <c:v>4.0</c:v>
+              </c:pt>
+              <c:pt idx="28">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="29">
+                <c:v>6.0</c:v>
+              </c:pt>
+              <c:pt idx="30">
+                <c:v>7.0</c:v>
+              </c:pt>
+              <c:pt idx="31">
+                <c:v>8.0</c:v>
+              </c:pt>
+              <c:pt idx="32">
+                <c:v>9.0</c:v>
+              </c:pt>
+              <c:pt idx="33">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="34">
+                <c:v>11.0</c:v>
+              </c:pt>
+              <c:pt idx="35">
+                <c:v>12.0</c:v>
+              </c:pt>
+              <c:pt idx="36">
+                <c:v>2017.1</c:v>
+              </c:pt>
+              <c:pt idx="37">
+                <c:v>2.0</c:v>
+              </c:pt>
+              <c:pt idx="38">
+                <c:v>3.0</c:v>
+              </c:pt>
+              <c:pt idx="39">
+                <c:v>4.0</c:v>
+              </c:pt>
+              <c:pt idx="40">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="41">
+                <c:v>6.0</c:v>
+              </c:pt>
+              <c:pt idx="42">
+                <c:v>7.0</c:v>
+              </c:pt>
+              <c:pt idx="43">
+                <c:v>8.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$A$43:$A$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>361.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>328.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>349.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>320.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>312.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>306.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>315.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>284.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>310.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>319.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>323.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>352.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>338.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>302.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>463.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3274.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1512.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1516.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1420.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1239.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1709.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1490.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1532.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1461.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1599.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1696.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1815.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2055.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1694.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1696.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1682.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1835.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2171.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3893.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3356.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2946.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2995.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3143.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3669.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4438.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4431.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4212.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3920.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3081.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="44"/>
+              <c:pt idx="0">
+                <c:v>2014.1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>2.0</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>3.0</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>4.0</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>6.0</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>7.0</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>8.0</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>9.0</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>11.0</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>12.0</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>2015.1</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>2.0</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>3.0</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>4.0</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>6.0</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>7.0</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>8.0</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>9.0</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>11.0</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>12.0</c:v>
+              </c:pt>
+              <c:pt idx="24">
+                <c:v>2016.1</c:v>
+              </c:pt>
+              <c:pt idx="25">
+                <c:v>2.0</c:v>
+              </c:pt>
+              <c:pt idx="26">
+                <c:v>3.0</c:v>
+              </c:pt>
+              <c:pt idx="27">
+                <c:v>4.0</c:v>
+              </c:pt>
+              <c:pt idx="28">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="29">
+                <c:v>6.0</c:v>
+              </c:pt>
+              <c:pt idx="30">
+                <c:v>7.0</c:v>
+              </c:pt>
+              <c:pt idx="31">
+                <c:v>8.0</c:v>
+              </c:pt>
+              <c:pt idx="32">
+                <c:v>9.0</c:v>
+              </c:pt>
+              <c:pt idx="33">
+                <c:v>10.0</c:v>
+              </c:pt>
+              <c:pt idx="34">
+                <c:v>11.0</c:v>
+              </c:pt>
+              <c:pt idx="35">
+                <c:v>12.0</c:v>
+              </c:pt>
+              <c:pt idx="36">
+                <c:v>2017.1</c:v>
+              </c:pt>
+              <c:pt idx="37">
+                <c:v>2.0</c:v>
+              </c:pt>
+              <c:pt idx="38">
+                <c:v>3.0</c:v>
+              </c:pt>
+              <c:pt idx="39">
+                <c:v>4.0</c:v>
+              </c:pt>
+              <c:pt idx="40">
+                <c:v>5.0</c:v>
+              </c:pt>
+              <c:pt idx="41">
+                <c:v>6.0</c:v>
+              </c:pt>
+              <c:pt idx="42">
+                <c:v>7.0</c:v>
+              </c:pt>
+              <c:pt idx="43">
+                <c:v>8.0</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>工作表1!$B$43:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="44"/>
+                <c:pt idx="0">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>155.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2313.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>850.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>836.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>721.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>605.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>925.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>715.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>711.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>663.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>771.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>747.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>787.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>912.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>677.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>672.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>678.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>764.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>924.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2324.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1096.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>915.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>830.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1003.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1022.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>912.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>835.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>937.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1003.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>833.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-1640574256"/>
+        <c:axId val="-1653162160"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-1640574256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1653162160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1653162160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1640574256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1601,7 +1965,596 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2182,6 +3135,38 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>699166</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>59747</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="图表 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2189,12 +3174,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.12911</cdr:x>
-      <cdr:y>0.19956</cdr:y>
+      <cdr:x>0.17966</cdr:x>
+      <cdr:y>0.07696</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.82348</cdr:x>
-      <cdr:y>0.25835</cdr:y>
+      <cdr:x>0.92755</cdr:x>
+      <cdr:y>0.13575</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2203,8 +3188,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2032849" y="2061449"/>
-          <a:ext cx="10933044" cy="607391"/>
+          <a:off x="2784932" y="773815"/>
+          <a:ext cx="11592807" cy="591139"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2221,34 +3206,34 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2400"/>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1"/>
             <a:t>New Users</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" baseline="0"/>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1" baseline="0"/>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2400"/>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1"/>
             <a:t>Sign</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" baseline="0"/>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1" baseline="0"/>
             <a:t> up Russian Stackoverflow</a:t>
           </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400" b="1"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.13065</cdr:x>
-      <cdr:y>0.28287</cdr:y>
+      <cdr:x>0.17966</cdr:x>
+      <cdr:y>0.15695</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.82582</cdr:x>
-      <cdr:y>0.34167</cdr:y>
+      <cdr:x>0.92989</cdr:x>
+      <cdr:y>0.21575</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2257,8 +3242,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2057032" y="2922105"/>
-          <a:ext cx="10945672" cy="607391"/>
+          <a:off x="2784932" y="1578188"/>
+          <a:ext cx="11629079" cy="591241"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2337,22 +3322,197 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2400"/>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1"/>
             <a:t>New Users who already have</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" baseline="0"/>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1" baseline="0"/>
             <a:t> </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2400"/>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1"/>
             <a:t>Stackoverflow account Sign</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" baseline="0"/>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1" baseline="0"/>
             <a:t> up Russian Stackoverflow</a:t>
           </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400" b="1"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.05094</cdr:x>
+      <cdr:y>0.05211</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.79883</cdr:x>
+      <cdr:y>0.1109</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="文本框 1"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="804250" y="532512"/>
+          <a:ext cx="11806765" cy="600819"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="accent1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1"/>
+            <a:t>New Users</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1"/>
+            <a:t>Sign</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1" baseline="0"/>
+            <a:t> up Russian Stackoverflow</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400" b="1"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.05094</cdr:x>
+      <cdr:y>0.12961</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.80117</cdr:x>
+      <cdr:y>0.18841</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="文本框 2"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="804250" y="1324589"/>
+          <a:ext cx="11843706" cy="600921"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1"/>
+            <a:t>New Users who already have</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1"/>
+            <a:t>Stackoverflow account Sign</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="2400" b="1" baseline="0"/>
+            <a:t> up Russian Stackoverflow</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="2400" b="1"/>
         </a:p>
       </cdr:txBody>
     </cdr:sp>
@@ -2623,10 +3783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:B86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" zoomScale="69" workbookViewId="0">
-      <selection activeCell="Y25" sqref="Y25"/>
+    <sheetView tabSelected="1" topLeftCell="U24" zoomScale="60" workbookViewId="0">
+      <selection activeCell="AW55" sqref="AW55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2636,7 +3796,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -2652,7 +3812,7 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2660,7 +3820,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -2668,7 +3828,7 @@
         <v>2</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2676,7 +3836,7 @@
         <v>58</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2684,7 +3844,7 @@
         <v>154</v>
       </c>
       <c r="B7">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2692,7 +3852,7 @@
         <v>158</v>
       </c>
       <c r="B8">
-        <v>80</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -2700,15 +3860,15 @@
         <v>325</v>
       </c>
       <c r="B9">
-        <v>126</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B10">
-        <v>92</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -2716,7 +3876,7 @@
         <v>226</v>
       </c>
       <c r="B11">
-        <v>79</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -2724,7 +3884,7 @@
         <v>157</v>
       </c>
       <c r="B12">
-        <v>47</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -2732,7 +3892,7 @@
         <v>266</v>
       </c>
       <c r="B13">
-        <v>92</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -2740,7 +3900,7 @@
         <v>352</v>
       </c>
       <c r="B14">
-        <v>99</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -2748,7 +3908,7 @@
         <v>485</v>
       </c>
       <c r="B15">
-        <v>126</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -2756,7 +3916,7 @@
         <v>399</v>
       </c>
       <c r="B16">
-        <v>118</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -2764,15 +3924,15 @@
         <v>345</v>
       </c>
       <c r="B17">
-        <v>106</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B18">
-        <v>86</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -2780,7 +3940,7 @@
         <v>394</v>
       </c>
       <c r="B19">
-        <v>111</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -2788,7 +3948,7 @@
         <v>332</v>
       </c>
       <c r="B20">
-        <v>105</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -2796,7 +3956,7 @@
         <v>324</v>
       </c>
       <c r="B21">
-        <v>101</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -2804,7 +3964,7 @@
         <v>359</v>
       </c>
       <c r="B22">
-        <v>95</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -2812,7 +3972,7 @@
         <v>233</v>
       </c>
       <c r="B23">
-        <v>83</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -2820,7 +3980,7 @@
         <v>226</v>
       </c>
       <c r="B24">
-        <v>65</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -2828,7 +3988,7 @@
         <v>304</v>
       </c>
       <c r="B25">
-        <v>149</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -2836,7 +3996,7 @@
         <v>247</v>
       </c>
       <c r="B26">
-        <v>121</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -2844,7 +4004,7 @@
         <v>192</v>
       </c>
       <c r="B27">
-        <v>88</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -2852,7 +4012,7 @@
         <v>320</v>
       </c>
       <c r="B28">
-        <v>171</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -2860,7 +4020,7 @@
         <v>276</v>
       </c>
       <c r="B29">
-        <v>142</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -2868,7 +4028,7 @@
         <v>205</v>
       </c>
       <c r="B30">
-        <v>105</v>
+        <v>39</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -2876,7 +4036,7 @@
         <v>221</v>
       </c>
       <c r="B31">
-        <v>98</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -2884,7 +4044,7 @@
         <v>214</v>
       </c>
       <c r="B32">
-        <v>104</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -2892,7 +4052,7 @@
         <v>245</v>
       </c>
       <c r="B33">
-        <v>120</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -2900,7 +4060,7 @@
         <v>233</v>
       </c>
       <c r="B34">
-        <v>116</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -2908,7 +4068,7 @@
         <v>292</v>
       </c>
       <c r="B35">
-        <v>138</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
@@ -2916,7 +4076,7 @@
         <v>288</v>
       </c>
       <c r="B36">
-        <v>141</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
@@ -2924,7 +4084,7 @@
         <v>266</v>
       </c>
       <c r="B37">
-        <v>139</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
@@ -2932,15 +4092,15 @@
         <v>310</v>
       </c>
       <c r="B38">
-        <v>159</v>
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B39">
-        <v>168</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -2948,7 +4108,7 @@
         <v>352</v>
       </c>
       <c r="B40">
-        <v>175</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -2956,7 +4116,7 @@
         <v>386</v>
       </c>
       <c r="B41">
-        <v>193</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
@@ -2964,7 +4124,7 @@
         <v>361</v>
       </c>
       <c r="B42">
-        <v>134</v>
+        <v>73</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
@@ -2972,7 +4132,7 @@
         <v>361</v>
       </c>
       <c r="B43">
-        <v>162</v>
+        <v>84</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
@@ -2980,7 +4140,7 @@
         <v>328</v>
       </c>
       <c r="B44">
-        <v>157</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
@@ -2988,7 +4148,7 @@
         <v>349</v>
       </c>
       <c r="B45">
-        <v>151</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
@@ -2996,7 +4156,7 @@
         <v>320</v>
       </c>
       <c r="B46">
-        <v>136</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
@@ -3004,7 +4164,7 @@
         <v>312</v>
       </c>
       <c r="B47">
-        <v>141</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
@@ -3012,7 +4172,7 @@
         <v>306</v>
       </c>
       <c r="B48">
-        <v>135</v>
+        <v>59</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
@@ -3020,7 +4180,7 @@
         <v>315</v>
       </c>
       <c r="B49">
-        <v>145</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
@@ -3028,31 +4188,31 @@
         <v>284</v>
       </c>
       <c r="B50">
-        <v>114</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B51">
-        <v>134</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B52">
-        <v>146</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B53">
-        <v>128</v>
+        <v>55</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
@@ -3060,15 +4220,15 @@
         <v>352</v>
       </c>
       <c r="B54">
-        <v>136</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B55">
-        <v>127</v>
+        <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
@@ -3076,7 +4236,7 @@
         <v>302</v>
       </c>
       <c r="B56">
-        <v>122</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
@@ -3084,15 +4244,15 @@
         <v>463</v>
       </c>
       <c r="B57">
-        <v>251</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>3280</v>
+        <v>3274</v>
       </c>
       <c r="B58">
-        <v>2749</v>
+        <v>2313</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
@@ -3100,39 +4260,39 @@
         <v>1512</v>
       </c>
       <c r="B59">
-        <v>1119</v>
+        <v>850</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="B60">
-        <v>1109</v>
+        <v>836</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>1422</v>
+        <v>1420</v>
       </c>
       <c r="B61">
-        <v>986</v>
+        <v>721</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>1240</v>
+        <v>1239</v>
       </c>
       <c r="B62">
-        <v>874</v>
+        <v>605</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>1713</v>
+        <v>1709</v>
       </c>
       <c r="B63">
-        <v>1268</v>
+        <v>925</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
@@ -3140,143 +4300,183 @@
         <v>1490</v>
       </c>
       <c r="B64">
-        <v>1044</v>
+        <v>715</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="B65">
-        <v>1048</v>
+        <v>711</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>1464</v>
+        <v>1461</v>
       </c>
       <c r="B66">
-        <v>959</v>
+        <v>663</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>1606</v>
+        <v>1599</v>
       </c>
       <c r="B67">
-        <v>1126</v>
+        <v>771</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>1702</v>
+        <v>1696</v>
       </c>
       <c r="B68">
-        <v>1104</v>
+        <v>747</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>1841</v>
+        <v>1815</v>
       </c>
       <c r="B69">
-        <v>1169</v>
+        <v>787</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>2080</v>
+        <v>2055</v>
       </c>
       <c r="B70">
-        <v>1308</v>
+        <v>912</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>1715</v>
+        <v>1694</v>
       </c>
       <c r="B71">
-        <v>1000</v>
+        <v>677</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>1730</v>
+        <v>1696</v>
       </c>
       <c r="B72">
-        <v>1040</v>
+        <v>672</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>1733</v>
+        <v>1682</v>
       </c>
       <c r="B73">
-        <v>995</v>
+        <v>678</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>1928</v>
+        <v>1835</v>
       </c>
       <c r="B74">
-        <v>1108</v>
+        <v>764</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>2633</v>
+        <v>2171</v>
       </c>
       <c r="B75">
-        <v>1243</v>
+        <v>924</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>4367</v>
+        <v>3893</v>
       </c>
       <c r="B76">
-        <v>2695</v>
+        <v>2324</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>3360</v>
+        <v>3356</v>
       </c>
       <c r="B77">
-        <v>1452</v>
+        <v>1096</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>2948</v>
+        <v>2946</v>
       </c>
       <c r="B78">
-        <v>1193</v>
+        <v>915</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>3002</v>
+        <v>2995</v>
       </c>
       <c r="B79">
-        <v>1091</v>
+        <v>830</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>3155</v>
+        <v>3143</v>
       </c>
       <c r="B80">
-        <v>1235</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>1298</v>
+        <v>3669</v>
       </c>
       <c r="B81">
-        <v>477</v>
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>4438</v>
+      </c>
+      <c r="B82">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>4431</v>
+      </c>
+      <c r="B83">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>4212</v>
+      </c>
+      <c r="B84">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>3920</v>
+      </c>
+      <c r="B85">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>3081</v>
+      </c>
+      <c r="B86">
+        <v>833</v>
       </c>
     </row>
   </sheetData>

</xml_diff>